<commit_message>
RTU tree HTML rearrangement
</commit_message>
<xml_diff>
--- a/AngularClientApp/lang/fibertest_strings.xlsx
+++ b/AngularClientApp/lang/fibertest_strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsGitProjects\Fibertest\AngularClientApp\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3473153-4ED4-4EDF-BC7A-81006403850E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E063F5-16C3-4343-B2C4-173238CE4150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22275" yWindow="3855" windowWidth="20280" windowHeight="11385" xr2:uid="{A7D3CB50-0A18-4D34-8249-9890304C4FB8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A7D3CB50-0A18-4D34-8249-9890304C4FB8}"/>
   </bookViews>
   <sheets>
     <sheet name="fibertest" sheetId="5" r:id="rId1"/>
@@ -8023,8 +8023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414197DE-5D7D-415C-BB9E-1CF1298E8AD7}">
   <dimension ref="A1:C858"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A707" workbookViewId="0">
+      <selection activeCell="A720" sqref="A720"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
mat-table sort and filter
</commit_message>
<xml_diff>
--- a/AngularClientApp/lang/fibertest_strings.xlsx
+++ b/AngularClientApp/lang/fibertest_strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsGitProjects\Fibertest\AngularClientApp\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E44DE5-850B-4494-BDC1-A9EB02FB2F8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F5E2E5-9AA7-4299-8B0A-9D3D8D2E4F8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22905" yWindow="1905" windowWidth="20280" windowHeight="12510" xr2:uid="{A7D3CB50-0A18-4D34-8249-9890304C4FB8}"/>
+    <workbookView xWindow="2880" yWindow="945" windowWidth="20280" windowHeight="12510" xr2:uid="{A7D3CB50-0A18-4D34-8249-9890304C4FB8}"/>
   </bookViews>
   <sheets>
     <sheet name="fibertest" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2576" uniqueCount="2526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2588" uniqueCount="2538">
   <si>
     <t>Name</t>
   </si>
@@ -7618,6 +7618,42 @@
   </si>
   <si>
     <t>Удаление зоны &lt;{{0}}&gt;!</t>
+  </si>
+  <si>
+    <t>SID_Items_per_page</t>
+  </si>
+  <si>
+    <t>SID_Next_page</t>
+  </si>
+  <si>
+    <t>SID_Previous_page</t>
+  </si>
+  <si>
+    <t>Items per page</t>
+  </si>
+  <si>
+    <t>Next page</t>
+  </si>
+  <si>
+    <t>Previous page</t>
+  </si>
+  <si>
+    <t>of</t>
+  </si>
+  <si>
+    <t>SID_of</t>
+  </si>
+  <si>
+    <t>из</t>
+  </si>
+  <si>
+    <t>Предыдущая страница</t>
+  </si>
+  <si>
+    <t>Следующая страница</t>
+  </si>
+  <si>
+    <t>Строк на странице</t>
   </si>
 </sst>
 </file>
@@ -8021,10 +8057,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414197DE-5D7D-415C-BB9E-1CF1298E8AD7}">
-  <dimension ref="A1:C858"/>
+  <dimension ref="A1:C863"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C530" sqref="C530"/>
+    <sheetView tabSelected="1" topLeftCell="A845" workbookViewId="0">
+      <selection activeCell="A860" sqref="A860"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17470,6 +17506,50 @@
       </c>
       <c r="C858" t="s">
         <v>2525</v>
+      </c>
+    </row>
+    <row r="860" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A860" t="s">
+        <v>2526</v>
+      </c>
+      <c r="B860" t="s">
+        <v>2529</v>
+      </c>
+      <c r="C860" t="s">
+        <v>2537</v>
+      </c>
+    </row>
+    <row r="861" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A861" t="s">
+        <v>2527</v>
+      </c>
+      <c r="B861" t="s">
+        <v>2530</v>
+      </c>
+      <c r="C861" t="s">
+        <v>2536</v>
+      </c>
+    </row>
+    <row r="862" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A862" t="s">
+        <v>2528</v>
+      </c>
+      <c r="B862" t="s">
+        <v>2531</v>
+      </c>
+      <c r="C862" t="s">
+        <v>2535</v>
+      </c>
+    </row>
+    <row r="863" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A863" t="s">
+        <v>2533</v>
+      </c>
+      <c r="B863" t="s">
+        <v>2532</v>
+      </c>
+      <c r="C863" t="s">
+        <v>2534</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
monitoring queue on RTU is written in tmp file first and replaced later
</commit_message>
<xml_diff>
--- a/AngularClientApp/lang/fibertest_strings.xlsx
+++ b/AngularClientApp/lang/fibertest_strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsGitProjects\Fibertest\AngularClientApp\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F5E2E5-9AA7-4299-8B0A-9D3D8D2E4F8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8FE552-BBE6-4E6F-8618-64FBD390DBE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="945" windowWidth="20280" windowHeight="12510" xr2:uid="{A7D3CB50-0A18-4D34-8249-9890304C4FB8}"/>
+    <workbookView xWindow="-22545" yWindow="2115" windowWidth="20280" windowHeight="12510" xr2:uid="{A7D3CB50-0A18-4D34-8249-9890304C4FB8}"/>
   </bookViews>
   <sheets>
     <sheet name="fibertest" sheetId="5" r:id="rId1"/>
@@ -7638,15 +7638,9 @@
     <t>Previous page</t>
   </si>
   <si>
-    <t>of</t>
-  </si>
-  <si>
     <t>SID_of</t>
   </si>
   <si>
-    <t>из</t>
-  </si>
-  <si>
     <t>Предыдущая страница</t>
   </si>
   <si>
@@ -7654,6 +7648,12 @@
   </si>
   <si>
     <t>Строк на странице</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> of </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> из </t>
   </si>
 </sst>
 </file>
@@ -8060,7 +8060,7 @@
   <dimension ref="A1:C863"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A845" workbookViewId="0">
-      <selection activeCell="A860" sqref="A860"/>
+      <selection activeCell="C863" sqref="C863"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17516,7 +17516,7 @@
         <v>2529</v>
       </c>
       <c r="C860" t="s">
-        <v>2537</v>
+        <v>2535</v>
       </c>
     </row>
     <row r="861" spans="1:3" x14ac:dyDescent="0.25">
@@ -17527,7 +17527,7 @@
         <v>2530</v>
       </c>
       <c r="C861" t="s">
-        <v>2536</v>
+        <v>2534</v>
       </c>
     </row>
     <row r="862" spans="1:3" x14ac:dyDescent="0.25">
@@ -17538,18 +17538,18 @@
         <v>2531</v>
       </c>
       <c r="C862" t="s">
-        <v>2535</v>
+        <v>2533</v>
       </c>
     </row>
     <row r="863" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A863" t="s">
-        <v>2533</v>
+        <v>2532</v>
       </c>
       <c r="B863" t="s">
-        <v>2532</v>
+        <v>2536</v>
       </c>
       <c r="C863" t="s">
-        <v>2534</v>
+        <v>2537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>